<commit_message>
Corrected Figure 3 experimental data sheet names
</commit_message>
<xml_diff>
--- a/Source_Data_Fig_3.xlsx
+++ b/Source_Data_Fig_3.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmansour/Desktop/DropletDeformationPaper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmansour/Documents/GitHub/abp-deformable-droplet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A266D1-7D95-044D-A5A1-E6321C3DCFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7044BA-9889-D946-894F-DCA745E86823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21520" yWindow="3660" windowWidth="27240" windowHeight="23420" xr2:uid="{A3400378-1FB2-ED45-9CB7-1F0BE53B0CA0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Fig 3B" sheetId="1" r:id="rId1"/>
-    <sheet name="Fig 3D" sheetId="2" r:id="rId2"/>
+    <sheet name="Fig 3C" sheetId="1" r:id="rId1"/>
+    <sheet name="Fig 3E" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -97,10 +97,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +453,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1532,7 +1531,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>